<commit_message>
Done some tests and fine tuning.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Documents\UiPath\fwf-api-poc-dispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B031CC-CFE3-4EEA-94D2-340C9A3F4BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11755A55-0CDD-4868-9651-383742185492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="27285" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>Path to where the attachments are being saved. NOTE: change this acording to your case.</t>
   </si>
   <si>
-    <t>C:\Users\DariusDangi\Documents\UiPath\fwf-api-poc-dispatcher\Data\Input\</t>
-  </si>
-  <si>
     <t>BRE2_Message</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>OutputReportPath</t>
   </si>
   <si>
-    <t>C:\Users\DariusDangi\Documents\UiPath\fwf-api-poc-dispatcher\Data\Output\OutputReport.xlsx</t>
-  </si>
-  <si>
     <t>Path to where the output reports its saved. NOTE: change this acording to your case.</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>Couldn't find in the given animals.</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\Input\</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\Output\OutputReport.xlsx</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -697,7 +697,7 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>54</v>
@@ -705,29 +705,29 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
         <v>58</v>
-      </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Ready for first review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11755A55-0CDD-4868-9651-383742185492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9E8AAC-6C8D-4937-B6D1-84AA1556070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="27285" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="1110" windowWidth="23325" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -95,132 +95,184 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>fwf-api-poc-dispatcher</t>
+  </si>
+  <si>
+    <t>Api-POC-Queue</t>
+  </si>
+  <si>
+    <t>Api-POC</t>
+  </si>
+  <si>
+    <t>SendersEmail</t>
+  </si>
+  <si>
+    <t>A list of all viable senders email. NOTE: The string has to be split using the comma separator.</t>
+  </si>
+  <si>
+    <t>AllowedAnimals</t>
+  </si>
+  <si>
+    <t>dog,cat</t>
+  </si>
+  <si>
+    <t>A list of allowed animals.</t>
+  </si>
+  <si>
+    <t>BRE1_Message</t>
+  </si>
+  <si>
+    <t>Couldn't find any email sent by an valid sender.</t>
+  </si>
+  <si>
+    <t>PathToSavedAttachments</t>
+  </si>
+  <si>
+    <t>Path to where the attachments are being saved. NOTE: change this acording to your case.</t>
+  </si>
+  <si>
+    <t>BRE2_Message</t>
+  </si>
+  <si>
+    <t>Couldn't find in the given email any attachment with the name: {0}.</t>
+  </si>
+  <si>
+    <t>OutputReportPath</t>
+  </si>
+  <si>
+    <t>Path to where the output reports its saved. NOTE: change this acording to your case.</t>
+  </si>
+  <si>
+    <t>BRE3_Message</t>
+  </si>
+  <si>
+    <t>Couldn't find in the given animals.</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\Input\</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\OutputReport.xlsx</t>
+  </si>
+  <si>
+    <t>BRE1_MailSubject</t>
+  </si>
+  <si>
+    <t>BRE1_MailTo</t>
+  </si>
+  <si>
+    <t>BRE1_MailBody</t>
+  </si>
+  <si>
+    <t>darius.dangi@fwfcompany.com</t>
+  </si>
+  <si>
+    <t>FWF Dog API POC | Incorrect Sender</t>
+  </si>
+  <si>
+    <t>BRE2_MailTo</t>
+  </si>
+  <si>
+    <t>BRE2_MailSubject</t>
+  </si>
+  <si>
+    <t>BRE2_MailBody</t>
+  </si>
+  <si>
+    <t>FWF Dog API POC | Incorrect Attachment</t>
+  </si>
+  <si>
+    <t>Am intalnit urmatoarea eroare: Atasamentul nu este corect / nu exista! 
+Multumesc!</t>
+  </si>
+  <si>
+    <t>Am intalnit urmatoarea eroare: Nu am depistat niciun email trimis de sender-ul agreat! 
+Multumesc!</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>fwf-api-poc-dispatcher</t>
-  </si>
-  <si>
-    <t>Api-POC-Queue</t>
-  </si>
-  <si>
-    <t>Api-POC</t>
-  </si>
-  <si>
-    <t>SendersEmail</t>
-  </si>
-  <si>
-    <t>A list of all viable senders email. NOTE: The string has to be split using the comma separator.</t>
-  </si>
-  <si>
-    <t>AllowedAnimals</t>
-  </si>
-  <si>
-    <t>dog,cat</t>
-  </si>
-  <si>
-    <t>A list of allowed animals.</t>
-  </si>
-  <si>
-    <t>BRE1_Message</t>
-  </si>
-  <si>
-    <t>Couldn't find any email sent by an valid sender.</t>
-  </si>
-  <si>
-    <t>PathToSavedAttachments</t>
-  </si>
-  <si>
-    <t>Path to where the attachments are being saved. NOTE: change this acording to your case.</t>
-  </si>
-  <si>
-    <t>BRE2_Message</t>
-  </si>
-  <si>
-    <t>Couldn't find in the given email any attachment with the name: {0}.</t>
-  </si>
-  <si>
-    <t>OutputReportPath</t>
-  </si>
-  <si>
-    <t>Path to where the output reports its saved. NOTE: change this acording to your case.</t>
-  </si>
-  <si>
-    <t>BRE3_Message</t>
-  </si>
-  <si>
-    <t>Couldn't find in the given animals.</t>
-  </si>
-  <si>
-    <t>C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\Input\</t>
-  </si>
-  <si>
-    <t>C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\Output\OutputReport.xlsx</t>
+  </si>
+  <si>
+    <t>AttachmentName</t>
+  </si>
+  <si>
+    <t>Colegi.xlsx</t>
+  </si>
+  <si>
+    <t>The name of attachment to be looked after.</t>
+  </si>
+  <si>
+    <t>OutlookInputEmailAddress</t>
+  </si>
+  <si>
+    <t>Email Address used to send mail messages</t>
+  </si>
+  <si>
+    <t>ListOfSenders</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,6 +296,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,10 +320,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,8 +334,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,7 +653,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -639,10 +700,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -650,13 +711,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -665,7 +726,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -675,80 +736,142 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
         <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>60</v>
       </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1717,8 +1840,13 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{77968CED-B851-426C-8518-09AB4023ACE5}"/>
+    <hyperlink ref="B16" r:id="rId2" xr:uid="{2C9546A8-F907-4ACF-A34C-78F3F16F16B0}"/>
+    <hyperlink ref="B24" r:id="rId3" xr:uid="{155A9B2B-8458-4524-9211-433F52651A62}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1780,18 +1908,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1815,7 +1943,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1837,7 +1965,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1848,7 +1976,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1859,53 +1987,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2889,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2909,7 +3037,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2939,16 +3067,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Changed to acording to first code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9E8AAC-6C8D-4937-B6D1-84AA1556070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F31B8E-B8B4-4375-99FB-CE90D3826363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1110" windowWidth="23325" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -266,13 +266,64 @@
   </si>
   <si>
     <t>ListOfSenders</t>
+  </si>
+  <si>
+    <t>OutputReportSheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>The name of excel sheet that is used when it's created.</t>
+  </si>
+  <si>
+    <t>OutputReportColumns</t>
+  </si>
+  <si>
+    <t>Name,Email,Animal,Status</t>
+  </si>
+  <si>
+    <t>Column names that are used to create the output report.</t>
+  </si>
+  <si>
+    <t>AttachmentSheetName</t>
+  </si>
+  <si>
+    <t>Name of used sheet in excel file</t>
+  </si>
+  <si>
+    <t>These are the keys that are going to be used in the queue items.</t>
+  </si>
+  <si>
+    <t>SearchingForColumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal </t>
+  </si>
+  <si>
+    <t>We are going to search this column to see if it contains dog/cat.</t>
+  </si>
+  <si>
+    <t>DictionaryTransactionItemsColumns</t>
+  </si>
+  <si>
+    <t>DictionarySenderEmailColumn</t>
+  </si>
+  <si>
+    <t>SenderEmail</t>
+  </si>
+  <si>
+    <t>This is not part of transactionItem, so we have to use another value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name,Email,Animal </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -296,12 +347,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,11 +365,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,10 +378,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -774,7 +816,7 @@
       <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>65</v>
       </c>
     </row>
@@ -798,7 +840,7 @@
       <c r="A16" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -832,46 +874,106 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1840,13 +1942,8 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{77968CED-B851-426C-8518-09AB4023ACE5}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{2C9546A8-F907-4ACF-A34C-78F3F16F16B0}"/>
-    <hyperlink ref="B24" r:id="rId3" xr:uid="{155A9B2B-8458-4524-9211-433F52651A62}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3017,7 +3114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified files acording to second code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-api-poc-dispatcher\fwf-api-poc-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F31B8E-B8B4-4375-99FB-CE90D3826363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C77CA0-C9B5-4D88-9BD2-87593F3C4492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t xml:space="preserve">Name,Email,Animal </t>
+  </si>
+  <si>
+    <t>OutlookMailFolder</t>
+  </si>
+  <si>
+    <t>Inbox</t>
+  </si>
+  <si>
+    <t>It will look into this mail folder to read the mail messages.</t>
   </si>
 </sst>
 </file>
@@ -695,7 +704,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -940,56 +949,66 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" t="s">
-        <v>88</v>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
       </c>
     </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
         <v>93</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>94</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>